<commit_message>
Modificaciones finales segunda entrega
</commit_message>
<xml_diff>
--- a/Dataset/diccionario de datos.xlsx
+++ b/Dataset/diccionario de datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Science Proyects\ds-ecommerce\Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elias Actis Grosso\Documents\Elias\Personal\Capacitación\Data\Data Science - Coder\TP final\ds-ecommerce\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC9A4AE-9BA0-47B1-918A-25E1FF6F72EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B63FD27-3297-47A4-B48D-63CD41DEC252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>ecomm_order_id</t>
   </si>
@@ -219,21 +219,41 @@
     <t>Sucursal a donde se envió el producto por última vez</t>
   </si>
   <si>
-    <t>Tipo de datos</t>
-  </si>
-  <si>
     <t>Ubicación  geográfica: Longitud</t>
   </si>
   <si>
     <t>Ubicación  geográfica:  Latitud</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>Sexo del comprador</t>
+  </si>
+  <si>
+    <t>client_id</t>
+  </si>
+  <si>
+    <t>Id único del cliente</t>
+  </si>
+  <si>
+    <t>Si es a domicilio o punto de retiro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -261,8 +281,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,31 +564,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="2" width="60.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="29.1796875" customWidth="1"/>
+    <col min="2" max="2" width="60.1796875" customWidth="1"/>
+    <col min="3" max="3" width="19.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -575,7 +593,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -583,7 +601,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -591,7 +609,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -599,7 +617,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -607,7 +625,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -615,7 +633,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -623,7 +641,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -631,7 +649,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -639,7 +657,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -647,7 +665,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -655,7 +673,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -663,7 +681,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -671,7 +689,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -679,12 +697,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -692,7 +713,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -700,7 +721,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -708,7 +729,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -716,7 +737,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -724,7 +745,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -732,7 +753,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -740,7 +761,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -748,7 +769,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -756,7 +777,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -764,7 +785,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -772,7 +793,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -780,7 +801,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -788,7 +809,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -796,7 +817,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -804,28 +825,44 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>